<commit_message>
cotização por excel e baixando dados automaticamente
</commit_message>
<xml_diff>
--- a/resultados/cotacoes acao US.xlsx
+++ b/resultados/cotacoes acao US.xlsx
@@ -389,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1277,6 +1277,34 @@
         <v>73.94999694824219</v>
       </c>
     </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B64">
+        <v>410.7699890136719</v>
+      </c>
+      <c r="C64">
+        <v>67.41000366210938</v>
+      </c>
+      <c r="D64">
+        <v>74.02999877929688</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="2">
+        <v>44775</v>
+      </c>
+      <c r="B65">
+        <v>411.7550048828125</v>
+      </c>
+      <c r="C65">
+        <v>67.52999877929688</v>
+      </c>
+      <c r="D65">
+        <v>74.47000122070312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>